<commit_message>
✅ commit scenarii :
Update scenarii
</commit_message>
<xml_diff>
--- a/Analyse/Thomas/Scénarii de tests.xlsx
+++ b/Analyse/Thomas/Scénarii de tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Desktop/projetVerinHydrauliqueSNAPP2/testDeVerinSurBancHydraulique/Analyse/Thomas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87FB445-5E94-2944-89C2-0723F9027714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00948769-7F85-204C-86A0-B0B1AA2998D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{58C722E9-39F1-F748-8D58-99E14D8B333F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" xr2:uid="{58C722E9-39F1-F748-8D58-99E14D8B333F}"/>
   </bookViews>
   <sheets>
     <sheet name="Scénarii - F2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>Étapes</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>Il clique sur l'onglet "visualisation du banc"</t>
+  </si>
+  <si>
+    <t>Toutes les informations et données sont visible</t>
   </si>
 </sst>
 </file>
@@ -566,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52E87AA-275B-084D-B4E0-E7A527D74359}">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,56 +636,58 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="1">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
     </row>
     <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -690,29 +695,29 @@
     </row>
     <row r="14" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="1">
-        <v>4</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -720,27 +725,19 @@
     </row>
     <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="1">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B15:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ update scenarii :
Update des scenarii F2, F4, F5
</commit_message>
<xml_diff>
--- a/Analyse/Thomas/Scénarii de tests.xlsx
+++ b/Analyse/Thomas/Scénarii de tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Desktop/projetVerinHydrauliqueSNAPP2/testDeVerinSurBancHydraulique/Analyse/Thomas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBFB7314-7F35-C448-9429-3E1EC3B480D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F71F99-86A5-BD42-9526-8D667453425C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" xr2:uid="{58C722E9-39F1-F748-8D58-99E14D8B333F}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="3" xr2:uid="{58C722E9-39F1-F748-8D58-99E14D8B333F}"/>
   </bookViews>
   <sheets>
     <sheet name="Scénarii - F2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Étapes</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>Toutes les informations et données sont visible</t>
+  </si>
+  <si>
+    <t>Interface IHM</t>
+  </si>
+  <si>
+    <t>Le manipulateur clique sur l'application Qt et décide de lancer ou non un essai</t>
+  </si>
+  <si>
+    <t>Le manipulateur clique sur le bouton pour commencer un essai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les données sont visible par le manipulateur </t>
+  </si>
+  <si>
+    <t>Le manipulateur clique sur le bouton "courbe" pour voir les points de la courbe</t>
+  </si>
+  <si>
+    <t>Le manipulateur visualise la même courbe mais de type oscilloscope</t>
   </si>
 </sst>
 </file>
@@ -229,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +271,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -569,17 +590,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D52E87AA-275B-084D-B4E0-E7A527D74359}">
-  <dimension ref="B1:E18"/>
+  <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" customWidth="1"/>
+    <col min="3" max="3" width="83.6640625" customWidth="1"/>
     <col min="4" max="4" width="74.83203125" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" customWidth="1"/>
   </cols>
@@ -664,80 +685,29 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B14" s="1">
-        <v>4</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="1">
-        <v>2</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B18" s="1">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1081,17 +1051,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C00CEB30-7F6D-B848-9B48-1A992EF12D8F}">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="80.6640625" customWidth="1"/>
+    <col min="3" max="3" width="92.6640625" customWidth="1"/>
     <col min="4" max="4" width="74.83203125" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" customWidth="1"/>
   </cols>
@@ -1131,7 +1101,9 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
@@ -1139,7 +1111,9 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
@@ -1147,107 +1121,26 @@
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="1">
+      <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B18" s="1">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="1">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
💡 commit Scénarii et Diagramme:
Les scénarii sont "terminé" et création du diagramme de classe
</commit_message>
<xml_diff>
--- a/Analyse/Thomas/Scénarii de tests.xlsx
+++ b/Analyse/Thomas/Scénarii de tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Desktop/projetVerinHydrauliqueSNAPP2/testDeVerinSurBancHydraulique/Analyse/Thomas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F71F99-86A5-BD42-9526-8D667453425C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF607F1A-1F33-6D4C-B397-B747E07F17A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="3" xr2:uid="{58C722E9-39F1-F748-8D58-99E14D8B333F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Étapes</t>
   </si>
@@ -130,6 +130,24 @@
   </si>
   <si>
     <t>Le manipulateur visualise la même courbe mais de type oscilloscope</t>
+  </si>
+  <si>
+    <t>Paramétrage des acquisitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réception des choix par défaut du contrôleur </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permettre la modification de ceux-ci </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Permettre la modification des paramètre de la carte </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lecture des données </t>
   </si>
 </sst>
 </file>
@@ -261,6 +279,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,9 +292,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -607,12 +625,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="71" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -629,12 +647,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -657,12 +675,12 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
@@ -685,12 +703,12 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
@@ -715,10 +733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987377A3-A7CD-C146-A8C8-86EB681A9573}">
-  <dimension ref="B1:E19"/>
+  <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:E16"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,10 +750,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="71" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -752,16 +772,20 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
@@ -769,7 +793,9 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
@@ -777,107 +803,26 @@
       <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B14" s="1">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B15" s="1">
+      <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B18" s="1">
-        <v>2</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B19" s="1">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -902,12 +847,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="71" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -924,12 +869,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -982,12 +927,12 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
@@ -1054,7 +999,7 @@
   <dimension ref="B1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1068,12 +1013,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="71" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -1090,12 +1035,12 @@
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -1131,10 +1076,10 @@
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="4"/>
     </row>
   </sheetData>

</xml_diff>